<commit_message>
Updated code, ignore column name
</commit_message>
<xml_diff>
--- a/partners/Me & My partner.xlsx
+++ b/partners/Me & My partner.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
   <si>
     <t>My Github User</t>
   </si>
@@ -25,6 +28,12 @@
     <t>Jarkapat</t>
   </si>
   <si>
+    <t>SPCH55</t>
+  </si>
+  <si>
+    <t>Peerawit321</t>
+  </si>
+  <si>
     <t>greatthanaporn</t>
   </si>
   <si>
@@ -64,13 +73,22 @@
     <t>Dowmean</t>
   </si>
   <si>
-    <t>Adam-00</t>
+    <t>Anuwatkl65</t>
+  </si>
+  <si>
+    <t>0xOat</t>
+  </si>
+  <si>
+    <t>kengklaubu</t>
   </si>
   <si>
     <t>Kittiphod-ka</t>
   </si>
   <si>
-    <t>kaikunz</t>
+    <t>chaiwat007x</t>
+  </si>
+  <si>
+    <t>gusgusxs</t>
   </si>
   <si>
     <t>ArirakSA</t>
@@ -103,6 +121,9 @@
     <t>AntMod46</t>
   </si>
   <si>
+    <t>Pxngya</t>
+  </si>
+  <si>
     <t>Jxuu03</t>
   </si>
   <si>
@@ -121,43 +142,64 @@
     <t>Thananon52437</t>
   </si>
   <si>
+    <t>jessadakorn65</t>
+  </si>
+  <si>
+    <t>Nudtikan</t>
+  </si>
+  <si>
+    <t>ManYaiMark</t>
+  </si>
+  <si>
+    <t>Bantita22j</t>
+  </si>
+  <si>
+    <t>hippopoman1</t>
+  </si>
+  <si>
+    <t>ZillerDX</t>
+  </si>
+  <si>
+    <t>sippanun65ubu</t>
+  </si>
+  <si>
+    <t>itthiphat</t>
+  </si>
+  <si>
+    <t>nakab20000</t>
+  </si>
+  <si>
+    <t>Siltawee</t>
+  </si>
+  <si>
+    <t>Supakorn4623</t>
+  </si>
+  <si>
+    <t>Thanawit3009</t>
+  </si>
+  <si>
+    <t>WachirawitSaenGsri</t>
+  </si>
+  <si>
+    <t>wanthit2</t>
+  </si>
+  <si>
+    <t>gojo3301</t>
+  </si>
+  <si>
+    <t>skibidi-thitiwat</t>
+  </si>
+  <si>
     <t>PhodsawiM</t>
   </si>
   <si>
-    <t>hippopoman1</t>
-  </si>
-  <si>
-    <t>ZillerDX</t>
-  </si>
-  <si>
-    <t>sippanun65ubu</t>
-  </si>
-  <si>
-    <t>itthiphat</t>
-  </si>
-  <si>
-    <t>nakab20000</t>
-  </si>
-  <si>
-    <t>Siltawee</t>
-  </si>
-  <si>
-    <t>Supakorn4623</t>
-  </si>
-  <si>
-    <t>Thanawit3009</t>
-  </si>
-  <si>
-    <t>WachirawitSaenGsri</t>
-  </si>
-  <si>
-    <t>wanthit2</t>
-  </si>
-  <si>
-    <t>gojo3301</t>
-  </si>
-  <si>
-    <t>skibidi-thitiwat</t>
+    <t>bomnattawut</t>
+  </si>
+  <si>
+    <t>Phanumatlaloed</t>
+  </si>
+  <si>
+    <t>Pisit65</t>
   </si>
 </sst>
 </file>
@@ -192,11 +234,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -243,11 +285,11 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,11 +512,14 @@
   </cols>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
@@ -482,27 +527,32 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -515,10 +565,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -526,10 +576,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -537,10 +587,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -548,10 +598,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -559,10 +609,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -570,43 +620,51 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
         <v>11.0</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
         <v>12.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
         <v>13.0</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
         <v>14.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
@@ -614,10 +672,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
@@ -625,10 +683,10 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18">
@@ -636,10 +694,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
@@ -647,26 +705,29 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
         <v>19.0</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
         <v>20.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22">
@@ -674,10 +735,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
@@ -685,7 +746,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -694,20 +755,29 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1">
         <v>24.0</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1">
         <v>25.0</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>36</v>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27">
@@ -715,10 +785,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28">
@@ -726,10 +796,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29">
@@ -737,10 +807,10 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30">
@@ -748,10 +818,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31">
@@ -759,10 +829,10 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32">
@@ -770,20 +840,32 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1">
         <v>32.0</v>
       </c>
+      <c r="B33" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1">
         <v>33.0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35">

</xml_diff>